<commit_message>
fix: wrong note for training to job on recommendation
</commit_message>
<xml_diff>
--- a/data/lowonganpekerjaan.xlsx
+++ b/data/lowonganpekerjaan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FDA2BC-A6CD-48DE-8AD5-61037ACFD840}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E4C0BE-2EC0-4ACA-AD5E-F159AD13D6FE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12375" windowHeight="8460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="353">
   <si>
     <t>PT Tenma Cikarang Indonesia</t>
   </si>
@@ -955,10 +955,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Mengelola dan mengoordinasikan proyek kerja sama dengan provider sesuai target dan timeline, menyusun perencanaan proyek, melakukan monitoring progres, serta mengevaluasi hasil pelaksanaan. Selain itu, melakukan komunikasi dan negosiasi dengan mitra atau provider, mengelola tim agar implementasi proyek berjalan efektif, menyusun laporan proyek dan presentasi menggunakan PowerPoint dan Excel, serta memastikan pencapaian target proyek dan penjualan sesuai ketentuan perusahaan.
-</t>
-  </si>
-  <si>
     <t>Deskripsi Pekerjaan</t>
   </si>
   <si>
@@ -990,6 +986,129 @@
   </si>
   <si>
     <t>Membantu teknisi AC dalam pemasangan dan perbaikan</t>
+  </si>
+  <si>
+    <t>PT Gunanusa Eramandiri</t>
+  </si>
+  <si>
+    <t>PT Bussan Auto Finance (BAF)</t>
+  </si>
+  <si>
+    <t>TikTok Content Creator</t>
+  </si>
+  <si>
+    <t>PT. Surya Perdana Makmur</t>
+  </si>
+  <si>
+    <t>Admin Marketplace</t>
+  </si>
+  <si>
+    <t>Autoretro Lumenslight Bekasi (Yoong Motor Bekasi)</t>
+  </si>
+  <si>
+    <t>Teknisi Perlampuan Kendaraan</t>
+  </si>
+  <si>
+    <t>PT. Gree Electric Appliances</t>
+  </si>
+  <si>
+    <t>Helper (Teknisi)</t>
+  </si>
+  <si>
+    <t>PT. Prakarsa Alam Segar</t>
+  </si>
+  <si>
+    <t>Teknisi Pengelasan</t>
+  </si>
+  <si>
+    <t>PT. Bumimulia Indah Lestari</t>
+  </si>
+  <si>
+    <t>PT Sora Bakery Group</t>
+  </si>
+  <si>
+    <t>Floor Supervisor</t>
+  </si>
+  <si>
+    <t>Jak Coffee Tea</t>
+  </si>
+  <si>
+    <t>Graphic Designer</t>
+  </si>
+  <si>
+    <t>PT. Karabha Digdaya</t>
+  </si>
+  <si>
+    <t>Teknisi Elektro</t>
+  </si>
+  <si>
+    <t>Manajer Proyek</t>
+  </si>
+  <si>
+    <t>Bertanggung jawab mengelola dan mengoordinasikan proyek kerja sama dengan provider agar berjalan sesuai target dan timeline. Pekerjaan mencakup penyusunan perencanaan proyek, pemantauan progres, evaluasi hasil, serta pengelolaan komunikasi dan negosiasi dengan mitra. Posisi ini juga mengelola tim proyek, menyusun laporan dan presentasi menggunakan PowerPoint dan Excel, serta memastikan target proyek dan penjualan tercapai sesuai ketentuan perusahaan.</t>
+  </si>
+  <si>
+    <t>Spesialis Teknologi Informasi Lainnya</t>
+  </si>
+  <si>
+    <t>Melakukan pengembangan dan integrasi perangkat IoT, sensor industri, dan gateway, termasuk pengelolaan komunikasi perangkat menggunakan berbagai protokol industri. Pekerjaan meliputi perancangan sistem otomasi berbasis PLC/SCADA, integrasi data ke database dan dashboard, pengembangan skrip otomatisasi, penerapan solusi AI/ML sederhana, serta troubleshooting sistem IoT dan otomasi baik di lokasi maupun pabrik.</t>
+  </si>
+  <si>
+    <t>Spesialis Pemasaran Digital</t>
+  </si>
+  <si>
+    <t>Mengembangkan strategi dan rencana konten media sosial yang selaras dengan identitas merek perusahaan. Bertanggung jawab memproduksi, menulis, dan mengedit konten untuk berbagai platform, meningkatkan engagement audiens, mempromosikan kampanye digital, serta berperan langsung sebagai talent media sosial khususnya di TikTok dan Instagram.</t>
+  </si>
+  <si>
+    <t>Petugas Administrasi Penjualan</t>
+  </si>
+  <si>
+    <t>Mengelola aktivitas operasional marketplace mulai dari unggah produk, optimasi judul dan deskripsi, pengelolaan pesanan harian, pengecekan pembayaran, hingga pembaruan resi pengiriman. Posisi ini juga menangani komunikasi dengan pelanggan, pengelolaan stok bersama gudang, pemantauan performa toko, serta penyusunan laporan penjualan bulanan.</t>
+  </si>
+  <si>
+    <t>Mekanik Kendaraan Bermotor</t>
+  </si>
+  <si>
+    <t>Melakukan pemasangan, perawatan, dan perbaikan sistem perlampuan kendaraan. Pekerjaan mencakup pemeriksaan kelistrikan, diagnosis masalah lampu kendaraan, serta memastikan instalasi berjalan aman dan sesuai standar. Teknisi juga bekerja sama dalam tim bengkel dan menjaga kualitas hasil pekerjaan.</t>
+  </si>
+  <si>
+    <t>Membantu pelaksanaan servis dan perbaikan unit pendingin atau AC, termasuk kegiatan supervisi proyek dan uji coba commissioning. Posisi ini juga berkoordinasi dengan Authorized Service Center untuk memastikan kualitas layanan dan hasil pekerjaan sesuai standar perusahaan.</t>
+  </si>
+  <si>
+    <t>Melaksanakan pekerjaan pengelasan menggunakan berbagai metode seperti TIG/Argon, SMAW, dan GTAW pada material stainless steel. Pekerjaan meliputi pembacaan gambar teknik, penggunaan peralatan las dan potong, serta memastikan hasil pengelasan memenuhi standar kualitas dan keselamatan kerja.</t>
+  </si>
+  <si>
+    <t>Teknisi Maintenance &amp; Utility</t>
+  </si>
+  <si>
+    <t>Teknisi Perawatan Mesin</t>
+  </si>
+  <si>
+    <t>Melakukan inspeksi rutin terhadap mesin produksi dan utilitas, menjalankan preventive dan corrective maintenance, serta mengganti komponen yang diperlukan. Teknisi juga memberikan pelatihan kepada operator produksi untuk meningkatkan kepedulian terhadap pemeliharaan mesin dan memastikan kelancaran operasional pabrik.</t>
+  </si>
+  <si>
+    <t>Supervisor Penjualan Ritel</t>
+  </si>
+  <si>
+    <t>Memimpin dan mengawasi operasional harian area hall bakery, termasuk pengaturan tim, pelayanan pelanggan, dan pencapaian target penjualan bersama Store Manager. Bertanggung jawab atas kebersihan, display produk, pelaporan berkala, serta menjaga hubungan baik dengan pihak mall.</t>
+  </si>
+  <si>
+    <t>Desainer Grafis</t>
+  </si>
+  <si>
+    <t>Bertanggung jawab menghasilkan visual yang konsisten dan relevan untuk seluruh kebutuhan branding dan pemasaran. Pekerjaan mencakup pengembangan identitas visual, konsep kreatif kampanye, desain kemasan dan merchandise, digital imaging produk, serta pembuatan aset desain offline untuk berbagai unit brand perusahaan.</t>
+  </si>
+  <si>
+    <t>Peracik Minuman</t>
+  </si>
+  <si>
+    <t>Menyiapkan dan menyajikan minuman kopi dan non-kopi sesuai standar, memberikan pelayanan pelanggan yang ramah dan profesional, menjaga kebersihan area kerja dan peralatan, serta mengelola stok bahan baku agar operasional kedai berjalan lancar.</t>
+  </si>
+  <si>
+    <t>PT. Megah Sakti Singosari</t>
+  </si>
+  <si>
+    <t>Melakukan instalasi, perawatan, dan perbaikan sistem kelistrikan, termasuk analisis gangguan dan pengujian peralatan. Bertanggung jawab memastikan pekerjaan sesuai standar keselamatan, menyusun laporan teknis, serta mendukung pengadaan suku cadang dan perlengkapan listrik.</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1158,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1052,8 +1171,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1089,22 +1214,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1164,14 +1278,35 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1390,8 +1525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBCCBE4D-47B2-4F57-828F-E7FDA402A59C}">
   <dimension ref="A1:G922"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,16 +1548,16 @@
         <v>93</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>95</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G1" s="15" t="s">
         <v>94</v>
@@ -2158,7 +2293,7 @@
         <v>152</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G33" s="20">
         <v>18</v>
@@ -3006,7 +3141,7 @@
         <v>2142</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F70" s="10" t="s">
         <v>253</v>
@@ -3029,7 +3164,7 @@
         <v>2151</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F71" s="10" t="s">
         <v>254</v>
@@ -3320,7 +3455,7 @@
         <v>3512</v>
       </c>
       <c r="E84" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F84" s="19" t="s">
         <v>267</v>
@@ -3596,7 +3731,7 @@
         <v>2431</v>
       </c>
       <c r="E96" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F96" s="18" t="s">
         <v>279</v>
@@ -3734,7 +3869,7 @@
         <v>2512</v>
       </c>
       <c r="E102" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F102" s="18" t="s">
         <v>285</v>
@@ -3757,7 +3892,7 @@
         <v>2163</v>
       </c>
       <c r="E103" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F103" s="18" t="s">
         <v>286</v>
@@ -3774,7 +3909,7 @@
         <v>36</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D104" s="11">
         <v>3119</v>
@@ -4065,7 +4200,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A117" s="9">
         <v>122</v>
       </c>
@@ -4084,11 +4219,11 @@
       <c r="F117" s="18" t="s">
         <v>300</v>
       </c>
-      <c r="G117" s="13">
+      <c r="G117" s="22">
         <v>25</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A118" s="9">
         <v>123</v>
       </c>
@@ -4098,95 +4233,326 @@
       <c r="C118" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="D118" s="11"/>
-      <c r="E118" s="12"/>
+      <c r="D118" s="11">
+        <v>2421</v>
+      </c>
+      <c r="E118" s="12" t="s">
+        <v>330</v>
+      </c>
       <c r="F118" s="18" t="s">
-        <v>301</v>
-      </c>
-      <c r="G118" s="13">
+        <v>331</v>
+      </c>
+      <c r="G118" s="22">
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="21"/>
-      <c r="B119" s="21"/>
-      <c r="C119" s="22"/>
-      <c r="D119" s="23"/>
-      <c r="G119" s="6"/>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G120" s="6"/>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G121" s="6"/>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G122" s="6"/>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G123" s="6"/>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G124" s="6"/>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G125" s="6"/>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G126" s="6"/>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G127" s="6"/>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G128" s="6"/>
-    </row>
-    <row r="129" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G129" s="6"/>
-    </row>
-    <row r="130" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A119" s="23">
+        <v>124</v>
+      </c>
+      <c r="B119" s="23" t="s">
+        <v>312</v>
+      </c>
+      <c r="C119" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D119" s="25">
+        <v>2529</v>
+      </c>
+      <c r="E119" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="F119" s="27" t="s">
+        <v>333</v>
+      </c>
+      <c r="G119" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A120" s="23">
+        <v>125</v>
+      </c>
+      <c r="B120" s="27" t="s">
+        <v>313</v>
+      </c>
+      <c r="C120" s="27" t="s">
+        <v>314</v>
+      </c>
+      <c r="D120" s="25">
+        <v>2432</v>
+      </c>
+      <c r="E120" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="F120" s="27" t="s">
+        <v>335</v>
+      </c>
+      <c r="G120" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A121" s="23">
+        <v>126</v>
+      </c>
+      <c r="B121" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="C121" s="27" t="s">
+        <v>316</v>
+      </c>
+      <c r="D121" s="25">
+        <v>3322</v>
+      </c>
+      <c r="E121" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="F121" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="G121" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A122" s="23">
+        <v>127</v>
+      </c>
+      <c r="B122" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="C122" s="27" t="s">
+        <v>318</v>
+      </c>
+      <c r="D122" s="25">
+        <v>7231</v>
+      </c>
+      <c r="E122" s="26" t="s">
+        <v>338</v>
+      </c>
+      <c r="F122" s="29" t="s">
+        <v>339</v>
+      </c>
+      <c r="G122" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A123" s="23">
+        <v>128</v>
+      </c>
+      <c r="B123" s="27" t="s">
+        <v>319</v>
+      </c>
+      <c r="C123" s="27" t="s">
+        <v>320</v>
+      </c>
+      <c r="D123" s="25">
+        <v>7126</v>
+      </c>
+      <c r="E123" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="F123" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="G123" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A124" s="23">
+        <v>129</v>
+      </c>
+      <c r="B124" s="27" t="s">
+        <v>321</v>
+      </c>
+      <c r="C124" s="27" t="s">
+        <v>322</v>
+      </c>
+      <c r="D124" s="25">
+        <v>7212</v>
+      </c>
+      <c r="E124" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="F124" s="27" t="s">
+        <v>341</v>
+      </c>
+      <c r="G124" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A125" s="23">
+        <v>130</v>
+      </c>
+      <c r="B125" s="27" t="s">
+        <v>323</v>
+      </c>
+      <c r="C125" s="27" t="s">
+        <v>342</v>
+      </c>
+      <c r="D125" s="25">
+        <v>7233</v>
+      </c>
+      <c r="E125" s="26" t="s">
+        <v>343</v>
+      </c>
+      <c r="F125" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="G125" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A126" s="23">
+        <v>131</v>
+      </c>
+      <c r="B126" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="C126" s="27" t="s">
+        <v>325</v>
+      </c>
+      <c r="D126" s="25">
+        <v>5222</v>
+      </c>
+      <c r="E126" s="26" t="s">
+        <v>345</v>
+      </c>
+      <c r="F126" s="27" t="s">
+        <v>346</v>
+      </c>
+      <c r="G126" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A127" s="23">
+        <v>132</v>
+      </c>
+      <c r="B127" s="27" t="s">
+        <v>326</v>
+      </c>
+      <c r="C127" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="D127" s="25">
+        <v>2166</v>
+      </c>
+      <c r="E127" s="26" t="s">
+        <v>347</v>
+      </c>
+      <c r="F127" s="27" t="s">
+        <v>348</v>
+      </c>
+      <c r="G127" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A128" s="23">
+        <v>133</v>
+      </c>
+      <c r="B128" s="27" t="s">
+        <v>328</v>
+      </c>
+      <c r="C128" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D128" s="25">
+        <v>5132</v>
+      </c>
+      <c r="E128" s="26" t="s">
+        <v>349</v>
+      </c>
+      <c r="F128" s="27" t="s">
+        <v>350</v>
+      </c>
+      <c r="G128" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A129" s="23">
+        <v>134</v>
+      </c>
+      <c r="B129" s="27" t="s">
+        <v>351</v>
+      </c>
+      <c r="C129" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="D129" s="25">
+        <v>7411</v>
+      </c>
+      <c r="E129" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="F129" s="27" t="s">
+        <v>352</v>
+      </c>
+      <c r="G129" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" s="30"/>
       <c r="G130" s="6"/>
     </row>
-    <row r="131" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" s="30"/>
       <c r="G131" s="6"/>
     </row>
-    <row r="132" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="30"/>
       <c r="G132" s="6"/>
     </row>
-    <row r="133" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" s="30"/>
       <c r="G133" s="6"/>
     </row>
-    <row r="134" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" s="30"/>
       <c r="G134" s="6"/>
     </row>
-    <row r="135" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="30"/>
       <c r="G135" s="6"/>
     </row>
-    <row r="136" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="30"/>
       <c r="G136" s="6"/>
     </row>
-    <row r="137" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="30"/>
       <c r="G137" s="6"/>
     </row>
-    <row r="138" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="30"/>
       <c r="G138" s="6"/>
     </row>
-    <row r="139" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" s="30"/>
       <c r="G139" s="6"/>
     </row>
-    <row r="140" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" s="30"/>
       <c r="G140" s="6"/>
     </row>
-    <row r="141" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G141" s="6"/>
     </row>
-    <row r="142" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G142" s="6"/>
     </row>
-    <row r="143" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G143" s="6"/>
     </row>
-    <row r="144" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G144" s="6"/>
     </row>
     <row r="145" spans="7:7" x14ac:dyDescent="0.25">

</xml_diff>